<commit_message>
# Testing color filling markers individually with different colors
</commit_message>
<xml_diff>
--- a/wafer-mapping-automation-test.xlsx
+++ b/wafer-mapping-automation-test.xlsx
@@ -2007,7 +2007,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2069,7 +2069,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3456,7 +3456,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -3518,7 +3518,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -4848,7 +4848,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -4910,7 +4910,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -6416,7 +6416,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -6478,7 +6478,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -6501,25 +6501,19 @@
       <tx>
         <rich>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-SG"/>
               <a:t>Scatter Chart Automation Test</a:t>
             </a:r>
           </a:p>
         </rich>
       </tx>
-      <overlay val="0"/>
     </title>
     <plotArea>
-      <layout/>
       <scatterChart>
-        <scatterStyle val="lineMarker"/>
-        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
@@ -6538,328 +6532,864 @@
               </a:ln>
             </spPr>
           </marker>
-          <xVal>
-            <numRef>
-              <f>'13th Wafer (ML RT 7)'!$C$2:$C$50</f>
-              <numCache>
-                <formatCode>General</formatCode>
-                <ptCount val="49"/>
-                <pt idx="0">
-                  <v>0</v>
-                </pt>
-                <pt idx="1">
-                  <v>32</v>
-                </pt>
-                <pt idx="2">
-                  <v>22.6273</v>
-                </pt>
-                <pt idx="3">
-                  <v>-0.0001</v>
-                </pt>
-                <pt idx="4">
-                  <v>-22.6275</v>
-                </pt>
-                <pt idx="5">
-                  <v>-32</v>
-                </pt>
-                <pt idx="6">
-                  <v>-22.6273</v>
-                </pt>
-                <pt idx="7">
-                  <v>0.0001</v>
-                </pt>
-                <pt idx="8">
-                  <v>22.6275</v>
-                </pt>
-                <pt idx="9">
-                  <v>64</v>
-                </pt>
-                <pt idx="10">
-                  <v>59.1282</v>
-                </pt>
-                <pt idx="11">
-                  <v>45.2547</v>
-                </pt>
-                <pt idx="12">
-                  <v>24.4915</v>
-                </pt>
-                <pt idx="13">
-                  <v>-0.0003</v>
-                </pt>
-                <pt idx="14">
-                  <v>-24.492</v>
-                </pt>
-                <pt idx="15">
-                  <v>-45.255</v>
-                </pt>
-                <pt idx="16">
-                  <v>-59.1284</v>
-                </pt>
-                <pt idx="17">
-                  <v>-64</v>
-                </pt>
-                <pt idx="18">
-                  <v>-59.1282</v>
-                </pt>
-                <pt idx="19">
-                  <v>-45.2547</v>
-                </pt>
-                <pt idx="20">
-                  <v>-24.4915</v>
-                </pt>
-                <pt idx="21">
-                  <v>0.0003</v>
-                </pt>
-                <pt idx="22">
-                  <v>24.492</v>
-                </pt>
-                <pt idx="23">
-                  <v>45.2551</v>
-                </pt>
-                <pt idx="24">
-                  <v>59.1284</v>
-                </pt>
-                <pt idx="25">
-                  <v>96</v>
-                </pt>
-                <pt idx="26">
-                  <v>92.72880000000001</v>
-                </pt>
-                <pt idx="27">
-                  <v>83.1383</v>
-                </pt>
-                <pt idx="28">
-                  <v>67.88200000000001</v>
-                </pt>
-                <pt idx="29">
-                  <v>47.9997</v>
-                </pt>
-                <pt idx="30">
-                  <v>24.8462</v>
-                </pt>
-                <pt idx="31">
-                  <v>-0.0004</v>
-                </pt>
-                <pt idx="32">
-                  <v>-24.847</v>
-                </pt>
-                <pt idx="33">
-                  <v>-48.0003</v>
-                </pt>
-                <pt idx="34">
-                  <v>-67.8826</v>
-                </pt>
-                <pt idx="35">
-                  <v>-83.1386</v>
-                </pt>
-                <pt idx="36">
-                  <v>-92.729</v>
-                </pt>
-                <pt idx="37">
-                  <v>-96</v>
-                </pt>
-                <pt idx="38">
-                  <v>-92.72880000000001</v>
-                </pt>
-                <pt idx="39">
-                  <v>-83.1382</v>
-                </pt>
-                <pt idx="40">
-                  <v>-67.88200000000001</v>
-                </pt>
-                <pt idx="41">
-                  <v>-47.9996</v>
-                </pt>
-                <pt idx="42">
-                  <v>-24.8462</v>
-                </pt>
-                <pt idx="43">
-                  <v>0.0004</v>
-                </pt>
-                <pt idx="44">
-                  <v>24.847</v>
-                </pt>
-                <pt idx="45">
-                  <v>48.0004</v>
-                </pt>
-                <pt idx="46">
-                  <v>67.8826</v>
-                </pt>
-                <pt idx="47">
-                  <v>83.1387</v>
-                </pt>
-                <pt idx="48">
-                  <v>92.729</v>
-                </pt>
-              </numCache>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'13th Wafer (ML RT 7)'!$B$2:$B$50</f>
-              <numCache>
-                <formatCode>General</formatCode>
-                <ptCount val="49"/>
-                <pt idx="0">
-                  <v>0</v>
-                </pt>
-                <pt idx="1">
-                  <v>-0.0001</v>
-                </pt>
-                <pt idx="2">
-                  <v>-22.6275</v>
-                </pt>
-                <pt idx="3">
-                  <v>-32</v>
-                </pt>
-                <pt idx="4">
-                  <v>-22.6273</v>
-                </pt>
-                <pt idx="5">
-                  <v>0.0001</v>
-                </pt>
-                <pt idx="6">
-                  <v>22.6275</v>
-                </pt>
-                <pt idx="7">
-                  <v>32</v>
-                </pt>
-                <pt idx="8">
-                  <v>22.6273</v>
-                </pt>
-                <pt idx="9">
-                  <v>-0.0002</v>
-                </pt>
-                <pt idx="10">
-                  <v>-24.492</v>
-                </pt>
-                <pt idx="11">
-                  <v>-45.255</v>
-                </pt>
-                <pt idx="12">
-                  <v>-59.1284</v>
-                </pt>
-                <pt idx="13">
-                  <v>-64</v>
-                </pt>
-                <pt idx="14">
-                  <v>-59.1282</v>
-                </pt>
-                <pt idx="15">
-                  <v>-45.2547</v>
-                </pt>
-                <pt idx="16">
-                  <v>-24.4915</v>
-                </pt>
-                <pt idx="17">
-                  <v>0.0003</v>
-                </pt>
-                <pt idx="18">
-                  <v>24.492</v>
-                </pt>
-                <pt idx="19">
-                  <v>45.2551</v>
-                </pt>
-                <pt idx="20">
-                  <v>59.1284</v>
-                </pt>
-                <pt idx="21">
-                  <v>64</v>
-                </pt>
-                <pt idx="22">
-                  <v>59.1282</v>
-                </pt>
-                <pt idx="23">
-                  <v>45.2546</v>
-                </pt>
-                <pt idx="24">
-                  <v>24.4915</v>
-                </pt>
-                <pt idx="25">
-                  <v>-0.0004</v>
-                </pt>
-                <pt idx="26">
-                  <v>-24.847</v>
-                </pt>
-                <pt idx="27">
-                  <v>-48.0003</v>
-                </pt>
-                <pt idx="28">
-                  <v>-67.88249999999999</v>
-                </pt>
-                <pt idx="29">
-                  <v>-83.1386</v>
-                </pt>
-                <pt idx="30">
-                  <v>-92.729</v>
-                </pt>
-                <pt idx="31">
-                  <v>-96</v>
-                </pt>
-                <pt idx="32">
-                  <v>-92.72880000000001</v>
-                </pt>
-                <pt idx="33">
-                  <v>-83.1382</v>
-                </pt>
-                <pt idx="34">
-                  <v>-67.88200000000001</v>
-                </pt>
-                <pt idx="35">
-                  <v>-47.9996</v>
-                </pt>
-                <pt idx="36">
-                  <v>-24.8462</v>
-                </pt>
-                <pt idx="37">
-                  <v>0.0004</v>
-                </pt>
-                <pt idx="38">
-                  <v>24.847</v>
-                </pt>
-                <pt idx="39">
-                  <v>48.0004</v>
-                </pt>
-                <pt idx="40">
-                  <v>67.8826</v>
-                </pt>
-                <pt idx="41">
-                  <v>83.1387</v>
-                </pt>
-                <pt idx="42">
-                  <v>92.729</v>
-                </pt>
-                <pt idx="43">
-                  <v>96</v>
-                </pt>
-                <pt idx="44">
-                  <v>92.72880000000001</v>
-                </pt>
-                <pt idx="45">
-                  <v>83.1382</v>
-                </pt>
-                <pt idx="46">
-                  <v>67.88200000000001</v>
-                </pt>
-                <pt idx="47">
-                  <v>47.9996</v>
-                </pt>
-                <pt idx="48">
-                  <v>24.8462</v>
-                </pt>
-              </numCache>
-            </numRef>
-          </yVal>
-          <smooth val="0"/>
+          <dPt>
+            <idx val="5"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="800000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
         </ser>
-        <dLbls>
-          <showLegendKey val="0"/>
-          <showVal val="0"/>
-          <showCatName val="0"/>
-          <showSerName val="0"/>
-          <showPercent val="0"/>
-          <showBubbleSize val="0"/>
-        </dLbls>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="9"/>
+          <order val="9"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="10"/>
+          <order val="10"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="11"/>
+          <order val="11"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="12"/>
+          <order val="12"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="13"/>
+          <order val="13"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="14"/>
+          <order val="14"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="15"/>
+          <order val="15"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="16"/>
+          <order val="16"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="17"/>
+          <order val="17"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="18"/>
+          <order val="18"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="19"/>
+          <order val="19"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="20"/>
+          <order val="20"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="21"/>
+          <order val="21"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="22"/>
+          <order val="22"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="23"/>
+          <order val="23"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="24"/>
+          <order val="24"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="25"/>
+          <order val="25"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="26"/>
+          <order val="26"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="27"/>
+          <order val="27"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="28"/>
+          <order val="28"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="29"/>
+          <order val="29"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="30"/>
+          <order val="30"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="31"/>
+          <order val="31"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="32"/>
+          <order val="32"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="33"/>
+          <order val="33"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="34"/>
+          <order val="34"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="35"/>
+          <order val="35"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="36"/>
+          <order val="36"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="37"/>
+          <order val="37"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="38"/>
+          <order val="38"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="39"/>
+          <order val="39"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="40"/>
+          <order val="40"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="41"/>
+          <order val="41"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="42"/>
+          <order val="42"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="43"/>
+          <order val="43"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="44"/>
+          <order val="44"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="45"/>
+          <order val="45"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="46"/>
+          <order val="46"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="47"/>
+          <order val="47"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="48"/>
+          <order val="48"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+        </ser>
+        <ser>
+          <idx val="49"/>
+          <order val="49"/>
+          <spPr>
+            <a:ln>
+              <a:noFill/>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="circle"/>
+            <size val="15"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <dPt>
+            <idx val="5"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="800000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
+        </ser>
         <axId val="10"/>
         <axId val="20"/>
       </scatterChart>
@@ -6868,32 +7398,22 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
-        <axPos val="b"/>
+        <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="20"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="midCat"/>
       </valAx>
       <valAx>
         <axId val="20"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="midCat"/>
       </valAx>
     </plotArea>
     <plotVisOnly val="1"/>
@@ -6909,25 +7429,19 @@
       <tx>
         <rich>
           <a:bodyPr/>
-          <a:lstStyle/>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-SG"/>
               <a:t>Scatter Chart Automation Test</a:t>
             </a:r>
           </a:p>
         </rich>
       </tx>
-      <overlay val="0"/>
     </title>
     <plotArea>
-      <layout/>
       <scatterChart>
-        <scatterStyle val="lineMarker"/>
-        <varyColors val="0"/>
         <ser>
           <idx val="0"/>
           <order val="0"/>
@@ -6946,328 +7460,28 @@
               </a:ln>
             </spPr>
           </marker>
+          <dPt>
+            <idx val="5"/>
+            <spPr>
+              <a:solidFill>
+                <a:srgbClr val="800000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </dPt>
           <xVal>
             <numRef>
               <f>'13th Wafer (ML RT 7)'!$C$2:$C$50</f>
-              <numCache>
-                <formatCode>General</formatCode>
-                <ptCount val="49"/>
-                <pt idx="0">
-                  <v>0</v>
-                </pt>
-                <pt idx="1">
-                  <v>32</v>
-                </pt>
-                <pt idx="2">
-                  <v>22.6273</v>
-                </pt>
-                <pt idx="3">
-                  <v>-0.0001</v>
-                </pt>
-                <pt idx="4">
-                  <v>-22.6275</v>
-                </pt>
-                <pt idx="5">
-                  <v>-32</v>
-                </pt>
-                <pt idx="6">
-                  <v>-22.6273</v>
-                </pt>
-                <pt idx="7">
-                  <v>0.0001</v>
-                </pt>
-                <pt idx="8">
-                  <v>22.6275</v>
-                </pt>
-                <pt idx="9">
-                  <v>64</v>
-                </pt>
-                <pt idx="10">
-                  <v>59.1282</v>
-                </pt>
-                <pt idx="11">
-                  <v>45.2547</v>
-                </pt>
-                <pt idx="12">
-                  <v>24.4915</v>
-                </pt>
-                <pt idx="13">
-                  <v>-0.0003</v>
-                </pt>
-                <pt idx="14">
-                  <v>-24.492</v>
-                </pt>
-                <pt idx="15">
-                  <v>-45.255</v>
-                </pt>
-                <pt idx="16">
-                  <v>-59.1284</v>
-                </pt>
-                <pt idx="17">
-                  <v>-64</v>
-                </pt>
-                <pt idx="18">
-                  <v>-59.1282</v>
-                </pt>
-                <pt idx="19">
-                  <v>-45.2547</v>
-                </pt>
-                <pt idx="20">
-                  <v>-24.4915</v>
-                </pt>
-                <pt idx="21">
-                  <v>0.0003</v>
-                </pt>
-                <pt idx="22">
-                  <v>24.492</v>
-                </pt>
-                <pt idx="23">
-                  <v>45.2551</v>
-                </pt>
-                <pt idx="24">
-                  <v>59.1284</v>
-                </pt>
-                <pt idx="25">
-                  <v>96</v>
-                </pt>
-                <pt idx="26">
-                  <v>92.72880000000001</v>
-                </pt>
-                <pt idx="27">
-                  <v>83.1383</v>
-                </pt>
-                <pt idx="28">
-                  <v>67.88200000000001</v>
-                </pt>
-                <pt idx="29">
-                  <v>47.9997</v>
-                </pt>
-                <pt idx="30">
-                  <v>24.8462</v>
-                </pt>
-                <pt idx="31">
-                  <v>-0.0004</v>
-                </pt>
-                <pt idx="32">
-                  <v>-24.847</v>
-                </pt>
-                <pt idx="33">
-                  <v>-48.0003</v>
-                </pt>
-                <pt idx="34">
-                  <v>-67.8826</v>
-                </pt>
-                <pt idx="35">
-                  <v>-83.1386</v>
-                </pt>
-                <pt idx="36">
-                  <v>-92.729</v>
-                </pt>
-                <pt idx="37">
-                  <v>-96</v>
-                </pt>
-                <pt idx="38">
-                  <v>-92.72880000000001</v>
-                </pt>
-                <pt idx="39">
-                  <v>-83.1382</v>
-                </pt>
-                <pt idx="40">
-                  <v>-67.88200000000001</v>
-                </pt>
-                <pt idx="41">
-                  <v>-47.9996</v>
-                </pt>
-                <pt idx="42">
-                  <v>-24.8462</v>
-                </pt>
-                <pt idx="43">
-                  <v>0.0004</v>
-                </pt>
-                <pt idx="44">
-                  <v>24.847</v>
-                </pt>
-                <pt idx="45">
-                  <v>48.0004</v>
-                </pt>
-                <pt idx="46">
-                  <v>67.8826</v>
-                </pt>
-                <pt idx="47">
-                  <v>83.1387</v>
-                </pt>
-                <pt idx="48">
-                  <v>92.729</v>
-                </pt>
-              </numCache>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
               <f>'13th Wafer (ML RT 7)'!$B$2:$B$50</f>
-              <numCache>
-                <formatCode>General</formatCode>
-                <ptCount val="49"/>
-                <pt idx="0">
-                  <v>0</v>
-                </pt>
-                <pt idx="1">
-                  <v>-0.0001</v>
-                </pt>
-                <pt idx="2">
-                  <v>-22.6275</v>
-                </pt>
-                <pt idx="3">
-                  <v>-32</v>
-                </pt>
-                <pt idx="4">
-                  <v>-22.6273</v>
-                </pt>
-                <pt idx="5">
-                  <v>0.0001</v>
-                </pt>
-                <pt idx="6">
-                  <v>22.6275</v>
-                </pt>
-                <pt idx="7">
-                  <v>32</v>
-                </pt>
-                <pt idx="8">
-                  <v>22.6273</v>
-                </pt>
-                <pt idx="9">
-                  <v>-0.0002</v>
-                </pt>
-                <pt idx="10">
-                  <v>-24.492</v>
-                </pt>
-                <pt idx="11">
-                  <v>-45.255</v>
-                </pt>
-                <pt idx="12">
-                  <v>-59.1284</v>
-                </pt>
-                <pt idx="13">
-                  <v>-64</v>
-                </pt>
-                <pt idx="14">
-                  <v>-59.1282</v>
-                </pt>
-                <pt idx="15">
-                  <v>-45.2547</v>
-                </pt>
-                <pt idx="16">
-                  <v>-24.4915</v>
-                </pt>
-                <pt idx="17">
-                  <v>0.0003</v>
-                </pt>
-                <pt idx="18">
-                  <v>24.492</v>
-                </pt>
-                <pt idx="19">
-                  <v>45.2551</v>
-                </pt>
-                <pt idx="20">
-                  <v>59.1284</v>
-                </pt>
-                <pt idx="21">
-                  <v>64</v>
-                </pt>
-                <pt idx="22">
-                  <v>59.1282</v>
-                </pt>
-                <pt idx="23">
-                  <v>45.2546</v>
-                </pt>
-                <pt idx="24">
-                  <v>24.4915</v>
-                </pt>
-                <pt idx="25">
-                  <v>-0.0004</v>
-                </pt>
-                <pt idx="26">
-                  <v>-24.847</v>
-                </pt>
-                <pt idx="27">
-                  <v>-48.0003</v>
-                </pt>
-                <pt idx="28">
-                  <v>-67.88249999999999</v>
-                </pt>
-                <pt idx="29">
-                  <v>-83.1386</v>
-                </pt>
-                <pt idx="30">
-                  <v>-92.729</v>
-                </pt>
-                <pt idx="31">
-                  <v>-96</v>
-                </pt>
-                <pt idx="32">
-                  <v>-92.72880000000001</v>
-                </pt>
-                <pt idx="33">
-                  <v>-83.1382</v>
-                </pt>
-                <pt idx="34">
-                  <v>-67.88200000000001</v>
-                </pt>
-                <pt idx="35">
-                  <v>-47.9996</v>
-                </pt>
-                <pt idx="36">
-                  <v>-24.8462</v>
-                </pt>
-                <pt idx="37">
-                  <v>0.0004</v>
-                </pt>
-                <pt idx="38">
-                  <v>24.847</v>
-                </pt>
-                <pt idx="39">
-                  <v>48.0004</v>
-                </pt>
-                <pt idx="40">
-                  <v>67.8826</v>
-                </pt>
-                <pt idx="41">
-                  <v>83.1387</v>
-                </pt>
-                <pt idx="42">
-                  <v>92.729</v>
-                </pt>
-                <pt idx="43">
-                  <v>96</v>
-                </pt>
-                <pt idx="44">
-                  <v>92.72880000000001</v>
-                </pt>
-                <pt idx="45">
-                  <v>83.1382</v>
-                </pt>
-                <pt idx="46">
-                  <v>67.88200000000001</v>
-                </pt>
-                <pt idx="47">
-                  <v>47.9996</v>
-                </pt>
-                <pt idx="48">
-                  <v>24.8462</v>
-                </pt>
-              </numCache>
             </numRef>
           </yVal>
-          <smooth val="0"/>
         </ser>
-        <dLbls>
-          <showLegendKey val="0"/>
-          <showVal val="0"/>
-          <showCatName val="0"/>
-          <showSerName val="0"/>
-          <showPercent val="0"/>
-          <showBubbleSize val="0"/>
-        </dLbls>
         <axId val="10"/>
         <axId val="20"/>
       </scatterChart>
@@ -7276,32 +7490,22 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
-        <axPos val="b"/>
+        <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="20"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="midCat"/>
       </valAx>
       <valAx>
         <axId val="20"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
-        <delete val="0"/>
         <axPos val="l"/>
         <majorGridlines/>
-        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="nextTo"/>
         <crossAx val="10"/>
-        <crosses val="autoZero"/>
-        <crossBetween val="midCat"/>
       </valAx>
     </plotArea>
     <plotVisOnly val="1"/>
@@ -8613,7 +8817,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -8675,7 +8879,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -9994,7 +10198,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -10056,7 +10260,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -11375,7 +11579,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -11437,7 +11641,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -12756,7 +12960,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -12818,7 +13022,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -14137,7 +14341,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -14199,7 +14403,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -15518,7 +15722,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -15580,7 +15784,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -16967,7 +17171,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -17029,7 +17233,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -18535,7 +18739,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -18597,7 +18801,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t/>
+              <a:t>None</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -23549,8 +23753,8 @@
   </sheetPr>
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
# Basic example for dynamically writing to each sheet name indicated by the wafer id
</commit_message>
<xml_diff>
--- a/wafer-mapping-automation-test.xlsx
+++ b/wafer-mapping-automation-test.xlsx
@@ -24832,7 +24832,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="49" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
@@ -25818,6 +25818,26 @@
       <c r="E50" s="9">
         <f>(D50*100)</f>
         <v/>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="36" t="n"/>
+      <c r="B85" s="36" t="n"/>
+      <c r="C85" s="36" t="n"/>
+      <c r="D85" s="36" t="inlineStr">
+        <is>
+          <t>mapitin</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="36" t="n"/>
+      <c r="B86" s="36" t="n"/>
+      <c r="C86" s="36" t="n"/>
+      <c r="D86" s="36" t="inlineStr">
+        <is>
+          <t>mapitin</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -30695,7 +30715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D11"/>
@@ -31703,6 +31723,22 @@
         <v>0</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" s="36" t="n"/>
+      <c r="B87" s="36" t="n"/>
+      <c r="C87" s="36" t="n"/>
+      <c r="D87" s="36" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="36" t="n"/>
+      <c r="B88" s="36" t="n"/>
+      <c r="C88" s="36" t="n"/>
+      <c r="D88" s="36" t="n">
+        <v>69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -31721,7 +31757,7 @@
   <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -33073,6 +33109,12 @@
         <f>PRODUCT(D38*100)</f>
         <v/>
       </c>
+      <c r="H38" s="9" t="n">
+        <v>-24.8462</v>
+      </c>
+      <c r="I38" s="9" t="n">
+        <v>-92.729</v>
+      </c>
       <c r="J38" t="n">
         <v>37</v>
       </c>
@@ -33106,6 +33148,12 @@
         <f>PRODUCT(D39*100)</f>
         <v/>
       </c>
+      <c r="H39" s="9" t="n">
+        <v>0.0004</v>
+      </c>
+      <c r="I39" s="9" t="n">
+        <v>-96</v>
+      </c>
       <c r="J39" t="n">
         <v>38</v>
       </c>
@@ -33139,6 +33187,12 @@
         <f>PRODUCT(D40*100)</f>
         <v/>
       </c>
+      <c r="H40" s="9" t="n">
+        <v>24.847</v>
+      </c>
+      <c r="I40" s="9" t="n">
+        <v>-92.72880000000001</v>
+      </c>
       <c r="J40" t="n">
         <v>39</v>
       </c>
@@ -33171,6 +33225,12 @@
       <c r="E41" s="9">
         <f>PRODUCT(D41*100)</f>
         <v/>
+      </c>
+      <c r="H41" s="9" t="n">
+        <v>48.0004</v>
+      </c>
+      <c r="I41" s="9" t="n">
+        <v>-83.1382</v>
       </c>
       <c r="J41" t="n">
         <v>40</v>

</xml_diff>